<commit_message>
Updated klassenvoorbeeld statistiek (with answers).
</commit_message>
<xml_diff>
--- a/klassenvoorbeeld_statistiek.xlsx
+++ b/klassenvoorbeeld_statistiek.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28227"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://hogeschoolutrecht-my.sharepoint.com/personal/tijmen_muller_hu_nl/Documents/workspace/vakken/Programming/klassen/24-V1S/demo/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tijmen.muller\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="255" documentId="8_{BD8611BD-EF25-40BD-956E-61DB8387B522}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4F105B6B-FD5E-41F1-ACD4-8ED855D3C015}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F3E23400-F915-456C-A731-14418B113E22}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{F69D1729-2F81-4851-9F8F-A83FB3A74BC5}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="50">
   <si>
     <t>Naam</t>
   </si>
@@ -180,6 +180,9 @@
   </si>
   <si>
     <t>categoriaal</t>
+  </si>
+  <si>
+    <t>check:</t>
   </si>
 </sst>
 </file>
@@ -188,7 +191,7 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="0.0%"/>
-    <numFmt numFmtId="168" formatCode="0.0"/>
+    <numFmt numFmtId="165" formatCode="0.0"/>
   </numFmts>
   <fonts count="6" x14ac:knownFonts="1">
     <font>
@@ -258,7 +261,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="5">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -312,6 +315,19 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color rgb="FFFF0000"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -319,7 +335,7 @@
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -335,7 +351,7 @@
     <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="2" applyBorder="1"/>
     <xf numFmtId="164" fontId="3" fillId="3" borderId="1" xfId="2" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="168" fontId="4" fillId="4" borderId="0" xfId="3" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="4" fillId="4" borderId="0" xfId="3" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
@@ -350,6 +366,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Bad" xfId="3" builtinId="27"/>
@@ -667,10 +684,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6F68A009-0DFA-426E-8BAB-14C1C2B99463}">
-  <dimension ref="A1:K1048576"/>
+  <dimension ref="A1:K1048569"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="F18" sqref="F18"/>
+    <sheetView tabSelected="1" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="B11" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="B1" sqref="B1"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="F23" sqref="F23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -986,6 +1006,14 @@
       <c r="G14" s="16">
         <v>158</v>
       </c>
+      <c r="H14">
+        <f t="shared" ref="H14:H21" si="0">G14-$B$25</f>
+        <v>-16.875</v>
+      </c>
+      <c r="I14">
+        <f>H14*H14</f>
+        <v>284.765625</v>
+      </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
@@ -1008,6 +1036,14 @@
       <c r="G15" s="16">
         <v>162</v>
       </c>
+      <c r="H15">
+        <f t="shared" si="0"/>
+        <v>-12.875</v>
+      </c>
+      <c r="I15">
+        <f t="shared" ref="I15:I21" si="1">H15*H15</f>
+        <v>165.765625</v>
+      </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
@@ -1030,8 +1066,16 @@
       <c r="G16" s="16">
         <v>172</v>
       </c>
-    </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="H16">
+        <f t="shared" si="0"/>
+        <v>-2.875</v>
+      </c>
+      <c r="I16">
+        <f t="shared" si="1"/>
+        <v>8.265625</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>17</v>
       </c>
@@ -1049,8 +1093,16 @@
         <f>E16+D17</f>
         <v>1</v>
       </c>
-      <c r="G17" s="16">
+      <c r="G17" s="20">
         <v>172</v>
+      </c>
+      <c r="H17">
+        <f t="shared" si="0"/>
+        <v>-2.875</v>
+      </c>
+      <c r="I17">
+        <f t="shared" si="1"/>
+        <v>8.265625</v>
       </c>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.25">
@@ -1073,6 +1125,14 @@
       </c>
       <c r="G18" s="16">
         <v>175</v>
+      </c>
+      <c r="H18">
+        <f t="shared" si="0"/>
+        <v>0.125</v>
+      </c>
+      <c r="I18">
+        <f t="shared" si="1"/>
+        <v>1.5625E-2</v>
       </c>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.25">
@@ -1080,131 +1140,187 @@
       <c r="G19" s="16">
         <v>182</v>
       </c>
+      <c r="H19">
+        <f t="shared" si="0"/>
+        <v>7.125</v>
+      </c>
+      <c r="I19">
+        <f t="shared" si="1"/>
+        <v>50.765625</v>
+      </c>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="G20" s="16">
         <v>185</v>
       </c>
+      <c r="H20">
+        <f t="shared" si="0"/>
+        <v>10.125</v>
+      </c>
+      <c r="I20">
+        <f t="shared" si="1"/>
+        <v>102.515625</v>
+      </c>
     </row>
     <row r="21" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="G21" s="17">
         <v>193</v>
       </c>
+      <c r="H21">
+        <f t="shared" si="0"/>
+        <v>18.125</v>
+      </c>
+      <c r="I21">
+        <f t="shared" si="1"/>
+        <v>328.515625</v>
+      </c>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A22" s="1"/>
-      <c r="B22" s="1" t="s">
+      <c r="F22" t="s">
+        <v>49</v>
+      </c>
+      <c r="G22">
+        <f>_xlfn.STDEV.P(G14:G21)</f>
+        <v>10.890793129979102</v>
+      </c>
+      <c r="I22">
+        <f>SUM(I14:I21)</f>
+        <v>948.875</v>
+      </c>
+      <c r="J22">
+        <f>I22/COUNT(I14:I21)</f>
+        <v>118.609375</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A24" s="1"/>
+      <c r="B24" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C22" s="1" t="s">
+      <c r="C24" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="D22" s="1" t="s">
+      <c r="D24" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="E22" s="1" t="s">
+      <c r="E24" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="F22" s="1" t="s">
+      <c r="F24" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="G22" s="1" t="s">
+      <c r="G24" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="H22" s="1" t="s">
+      <c r="H24" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="I22" s="1" t="s">
+      <c r="I24" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="J22" s="1" t="s">
+      <c r="J24" s="1" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A23" s="1" t="s">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A25" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B23" s="14">
+      <c r="B25" s="14">
         <f>SUM(C2:C9)/COUNT(C2:C9)</f>
         <v>174.875</v>
       </c>
-      <c r="C23" s="14">
+      <c r="C25" s="14">
         <v>172</v>
       </c>
-      <c r="D23" s="14">
+      <c r="D25" s="14">
         <v>173.5</v>
       </c>
-      <c r="E23" s="14"/>
-      <c r="F23" s="14"/>
-      <c r="G23" s="14"/>
-      <c r="H23" s="14"/>
-      <c r="I23" s="14"/>
-      <c r="J23" s="14"/>
-    </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A24" s="1" t="s">
+      <c r="E25" s="14">
+        <f>G21-G14</f>
+        <v>35</v>
+      </c>
+      <c r="F25" s="14">
+        <v>118.609375</v>
+      </c>
+      <c r="G25" s="14">
+        <f>SQRT(F25)</f>
+        <v>10.890793129979102</v>
+      </c>
+      <c r="H25" s="14">
+        <v>167</v>
+      </c>
+      <c r="I25" s="14">
+        <f>D25</f>
+        <v>173.5</v>
+      </c>
+      <c r="J25" s="14">
+        <v>183.5</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A26" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B24" s="14">
+      <c r="B26" s="14">
         <f>SUM(D2:D9)/COUNT(D2:D9)</f>
         <v>2003.125</v>
       </c>
-      <c r="C24" s="14" t="s">
+      <c r="C26" s="14" t="s">
         <v>37</v>
       </c>
-      <c r="D24" s="14"/>
-      <c r="E24" s="14"/>
-      <c r="F24" s="14"/>
-      <c r="G24" s="14"/>
-      <c r="H24" s="14"/>
-      <c r="I24" s="14"/>
-      <c r="J24" s="14"/>
-    </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A25" s="1" t="s">
+      <c r="D26" s="14"/>
+      <c r="E26" s="14"/>
+      <c r="F26" s="14"/>
+      <c r="G26" s="14"/>
+      <c r="H26" s="14"/>
+      <c r="I26" s="14"/>
+      <c r="J26" s="14"/>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A27" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B25" s="14">
+      <c r="B27" s="14">
         <f>SUM(E2:E9)/COUNT(E2:E9)</f>
         <v>41</v>
       </c>
-      <c r="C25" s="14" t="s">
+      <c r="C27" s="14" t="s">
         <v>36</v>
       </c>
-      <c r="D25" s="14"/>
-      <c r="E25" s="14"/>
-      <c r="F25" s="14"/>
-      <c r="G25" s="14"/>
-      <c r="H25" s="14"/>
-      <c r="I25" s="14"/>
-      <c r="J25" s="14"/>
-    </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A26" s="1" t="s">
+      <c r="D27" s="14"/>
+      <c r="E27" s="14"/>
+      <c r="F27" s="14"/>
+      <c r="G27" s="14"/>
+      <c r="H27" s="14"/>
+      <c r="I27" s="14"/>
+      <c r="J27" s="14"/>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A28" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B26" s="14" t="s">
+      <c r="B28" s="14" t="s">
         <v>35</v>
       </c>
-      <c r="C26" s="14" t="s">
+      <c r="C28" s="14" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A27" s="1" t="s">
+    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A29" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B27" s="13">
+      <c r="B29" s="13">
         <f>SUM(H2:H9)/COUNT(H2:H9)</f>
         <v>3.5</v>
       </c>
-      <c r="C27" s="14" t="s">
+      <c r="C29" s="14" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="1048576" spans="11:11" x14ac:dyDescent="0.25">
-      <c r="K1048576" t="s">
+    <row r="1048569" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K1048569" t="s">
         <v>17</v>
       </c>
     </row>

</xml_diff>